<commit_message>
Actualizacion de las tablas, y mantenimiento Representantes
</commit_message>
<xml_diff>
--- a/InventoryDoc.xlsx
+++ b/InventoryDoc.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximo j. herrera\Desktop\C# beginner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D57C816-28C9-4BBA-A610-E17F9B326274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBA7C2D-4DF6-48C6-A999-D90FE5EB88FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{943060A4-D9D7-47BF-8B1E-3AF7F048CD3B}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7270" activeTab="2" xr2:uid="{943060A4-D9D7-47BF-8B1E-3AF7F048CD3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="163">
   <si>
     <t>Suplidores</t>
   </si>
@@ -360,13 +360,172 @@
   </si>
   <si>
     <t>dotnet new blazor -o InventoryBlazor</t>
+  </si>
+  <si>
+    <t>Tablas</t>
+  </si>
+  <si>
+    <t>Realizados</t>
+  </si>
+  <si>
+    <t>Categorias</t>
+  </si>
+  <si>
+    <t>CategoriasId</t>
+  </si>
+  <si>
+    <t>Subcategorias</t>
+  </si>
+  <si>
+    <t>SubcategoriasId</t>
+  </si>
+  <si>
+    <t>Descripcon</t>
+  </si>
+  <si>
+    <t>CategoriaId</t>
+  </si>
+  <si>
+    <t>UnidadMedida</t>
+  </si>
+  <si>
+    <t>Recetas</t>
+  </si>
+  <si>
+    <t>RecetaId</t>
+  </si>
+  <si>
+    <t>DetalleReceta</t>
+  </si>
+  <si>
+    <t>DetalleRecetaId</t>
+  </si>
+  <si>
+    <t>EsProducto</t>
+  </si>
+  <si>
+    <t>EsIngrediente</t>
+  </si>
+  <si>
+    <t>EsUtensilo</t>
+  </si>
+  <si>
+    <t>FechaRegistro</t>
+  </si>
+  <si>
+    <t>Mermas</t>
+  </si>
+  <si>
+    <t>MermaId</t>
+  </si>
+  <si>
+    <t>Motivo</t>
+  </si>
+  <si>
+    <t>Lotes</t>
+  </si>
+  <si>
+    <t>FechaIngreso</t>
+  </si>
+  <si>
+    <t>FechaCaducidad</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>WHERE l.FechaCaducidad &lt;= DATEADD(DAY, 7, GETDATE())</t>
+  </si>
+  <si>
+    <t>SubcategoriaId</t>
+  </si>
+  <si>
+    <t>LoteId</t>
+  </si>
+  <si>
+    <t>DetalleReclamacion</t>
+  </si>
+  <si>
+    <t>Cajas</t>
+  </si>
+  <si>
+    <t>CajaId</t>
+  </si>
+  <si>
+    <t>LocalId</t>
+  </si>
+  <si>
+    <t>AperturaCaja</t>
+  </si>
+  <si>
+    <t>AperturaCajaId</t>
+  </si>
+  <si>
+    <t>UsuarioId</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>Movimientos</t>
+  </si>
+  <si>
+    <t>MovimientoId</t>
+  </si>
+  <si>
+    <t>AperturaId</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>NoTransaccion</t>
+  </si>
+  <si>
+    <t>CierreCaja</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
+  </si>
+  <si>
+    <t>Denominacion</t>
+  </si>
+  <si>
+    <t>DenominacionId</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>CierreCajaId</t>
+  </si>
+  <si>
+    <t>ArqueoApertura</t>
+  </si>
+  <si>
+    <t>ArqueoAperturaId</t>
+  </si>
+  <si>
+    <t>MovDenominacion</t>
+  </si>
+  <si>
+    <t>MovDenominacionId</t>
+  </si>
+  <si>
+    <t>ArqueoCierre</t>
+  </si>
+  <si>
+    <t>ArqueoCierreId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,8 +533,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +566,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -413,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -422,6 +594,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA29F8E-0666-4334-ADE8-7C214EB64214}">
-  <dimension ref="A1:A186"/>
+  <dimension ref="A1:B198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection sqref="A1:B207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -752,814 +926,869 @@
     <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" s="3" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A111" s="3" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" s="3" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" s="3" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A123" s="3" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" s="3" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" s="3" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A136" s="3" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" s="3" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A143" s="3" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" s="3" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1632,4 +1861,1292 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D113699-8150-41D8-BE08-29B9284B5EC5}">
+  <dimension ref="A1:B291"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A287" sqref="A287"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A201" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A207" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A215" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A222" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A230" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A239" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A245" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A253" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A263" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A270" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A275" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A281" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A284" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A287" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A289" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>